<commit_message>
Add table for man.grav method in UQ2, run code for this, gd and compare.
</commit_message>
<xml_diff>
--- a/experiments/UQ2/man.grav/UQ2_man_grav.xlsx
+++ b/experiments/UQ2/man.grav/UQ2_man_grav.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au521230\Documents\GitHub\GD-BMP\experiments\UQ2\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\au521230\Documents\GitHub\GD-BMP\experiments\UQ2\man.grav\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" tabRatio="855" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" tabRatio="855" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Setup_Mano_Grav" sheetId="1" r:id="rId1"/>
@@ -57,7 +57,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="387" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="87">
   <si>
     <t>id</t>
   </si>
@@ -309,6 +309,15 @@
   </si>
   <si>
     <t>Change name of comp in both sheets for CO2 and CH4 to cCH4 and cCO2</t>
+  </si>
+  <si>
+    <t>conc.sub.vs</t>
+  </si>
+  <si>
+    <t>conc.inoc.vs</t>
+  </si>
+  <si>
+    <t>Add conc.vs for inoc and sub</t>
   </si>
 </sst>
 </file>
@@ -929,10 +938,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K38"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
     <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="O9" sqref="O9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,11 +949,13 @@
     <col min="1" max="2" width="11.85546875" style="15" customWidth="1"/>
     <col min="3" max="3" width="14.140625" style="15" bestFit="1" customWidth="1"/>
     <col min="4" max="9" width="11.85546875" style="15" customWidth="1"/>
-    <col min="10" max="1018" width="8.5703125" style="15"/>
+    <col min="10" max="12" width="8.5703125" style="15"/>
+    <col min="13" max="13" width="11" style="15" bestFit="1" customWidth="1"/>
+    <col min="14" max="1018" width="8.5703125" style="15"/>
     <col min="1019" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="45" x14ac:dyDescent="0.25">
       <c r="A1" s="16" t="s">
         <v>26</v>
       </c>
@@ -979,7 +990,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="17" t="s">
         <v>0</v>
       </c>
@@ -1013,8 +1024,14 @@
       <c r="K2" s="15" t="s">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L2" s="15" t="s">
+        <v>84</v>
+      </c>
+      <c r="M2" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
         <v>73</v>
       </c>
@@ -1045,8 +1062,12 @@
       <c r="J3" s="21">
         <v>1.5212236591091561</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M3" s="15">
+        <f>J3/(D3*1000)</f>
+        <v>1.9006030299093645E-5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="15" t="s">
         <v>74</v>
       </c>
@@ -1077,8 +1098,12 @@
       <c r="J4" s="21">
         <v>1.5212236591091561</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M4" s="15">
+        <f t="shared" ref="M4:M11" si="0">J4/(D4*1000)</f>
+        <v>1.9006030299093645E-5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="15" t="s">
         <v>75</v>
       </c>
@@ -1109,8 +1134,12 @@
       <c r="J5" s="21">
         <v>1.5212236591091561</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="M5" s="15">
+        <f t="shared" si="0"/>
+        <v>1.9006030299093645E-5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="15" t="s">
         <v>43</v>
       </c>
@@ -1144,8 +1173,16 @@
       <c r="K6" s="21">
         <v>1.8335666567127771</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L6" s="15">
+        <f t="shared" ref="L4:L11" si="1">I6/(E6*1000)</f>
+        <v>9.7397515923315907E-4</v>
+      </c>
+      <c r="M6" s="15">
+        <f t="shared" si="0"/>
+        <v>1.9006030299093645E-5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="15" t="s">
         <v>44</v>
       </c>
@@ -1179,8 +1216,16 @@
       <c r="K7" s="21">
         <v>1.8335666567127771</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L7" s="15">
+        <f t="shared" si="1"/>
+        <v>9.7397515923315907E-4</v>
+      </c>
+      <c r="M7" s="15">
+        <f t="shared" si="0"/>
+        <v>1.9006030299093645E-5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="15" t="s">
         <v>45</v>
       </c>
@@ -1214,8 +1259,16 @@
       <c r="K8" s="21">
         <v>1.8335666567127771</v>
       </c>
-    </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L8" s="15">
+        <f t="shared" si="1"/>
+        <v>9.7397515923315907E-4</v>
+      </c>
+      <c r="M8" s="15">
+        <f t="shared" si="0"/>
+        <v>1.9006030299093645E-5</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="15" t="s">
         <v>7</v>
       </c>
@@ -1249,8 +1302,16 @@
       <c r="K9" s="21">
         <v>1.9278241310598954</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L9" s="15">
+        <f t="shared" si="1"/>
+        <v>8.130054802589125E-4</v>
+      </c>
+      <c r="M9" s="15">
+        <f t="shared" si="0"/>
+        <v>1.9006030299093642E-5</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="15" t="s">
         <v>9</v>
       </c>
@@ -1284,8 +1345,16 @@
       <c r="K10" s="21">
         <v>1.9278241310598954</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L10" s="15">
+        <f t="shared" si="1"/>
+        <v>8.130054802589125E-4</v>
+      </c>
+      <c r="M10" s="15">
+        <f t="shared" si="0"/>
+        <v>1.9006030299093642E-5</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="15" t="s">
         <v>10</v>
       </c>
@@ -1319,23 +1388,31 @@
       <c r="K11" s="21">
         <v>1.9278241310598954</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="L11" s="15">
+        <f t="shared" si="1"/>
+        <v>8.130054802589125E-4</v>
+      </c>
+      <c r="M11" s="15">
+        <f t="shared" si="0"/>
+        <v>1.9006030299093642E-5</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G12" s="18"/>
       <c r="H12" s="18"/>
       <c r="I12" s="20"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G13" s="18"/>
       <c r="H13" s="18"/>
       <c r="I13" s="20"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G14" s="18"/>
       <c r="H14" s="18"/>
       <c r="I14" s="20"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -1347,7 +1424,7 @@
       <c r="I15" s="16"/>
       <c r="J15" s="22"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="17"/>
       <c r="B16" s="17"/>
       <c r="C16" s="17"/>
@@ -1514,7 +1591,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M227"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B78" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -11737,8 +11814,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -11817,27 +11894,36 @@
         <v>80</v>
       </c>
     </row>
-    <row r="17" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D17" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C18" s="10"/>
     </row>
-    <row r="19" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="8" t="s">
+        <v>60</v>
+      </c>
       <c r="C19" s="10"/>
-    </row>
-    <row r="20" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="11" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C20" s="10"/>
     </row>
-    <row r="21" spans="3:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" s="11" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C21" s="10"/>
     </row>
-    <row r="22" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D22" s="14"/>
     </row>
-    <row r="24" spans="3:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D24" s="14"/>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add round function and adjustments of man.grav data for supplementary
</commit_message>
<xml_diff>
--- a/experiments/UQ2/man.grav/UQ2_man_grav.xlsx
+++ b/experiments/UQ2/man.grav/UQ2_man_grav.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" tabRatio="855" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21600" windowHeight="10185" tabRatio="855"/>
   </bookViews>
   <sheets>
     <sheet name="Setup_Mano_Grav" sheetId="1" r:id="rId1"/>
@@ -940,8 +940,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="O9" sqref="O9"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L16" sqref="L16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1063,8 +1063,8 @@
         <v>1.5212236591091561</v>
       </c>
       <c r="M3" s="15">
-        <f>J3/(D3*1000)</f>
-        <v>1.9006030299093645E-5</v>
+        <f>(1000*J3)/D3</f>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
@@ -1099,8 +1099,8 @@
         <v>1.5212236591091561</v>
       </c>
       <c r="M4" s="15">
-        <f t="shared" ref="M4:M11" si="0">J4/(D4*1000)</f>
-        <v>1.9006030299093645E-5</v>
+        <f t="shared" ref="M4:M11" si="0">(1000*J4)/D4</f>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
@@ -1136,7 +1136,7 @@
       </c>
       <c r="M5" s="15">
         <f t="shared" si="0"/>
-        <v>1.9006030299093645E-5</v>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
@@ -1174,12 +1174,12 @@
         <v>1.8335666567127771</v>
       </c>
       <c r="L6" s="15">
-        <f t="shared" ref="L4:L11" si="1">I6/(E6*1000)</f>
-        <v>9.7397515923315907E-4</v>
+        <f>(I6*1000)/E6</f>
+        <v>973.97515923315905</v>
       </c>
       <c r="M6" s="15">
         <f t="shared" si="0"/>
-        <v>1.9006030299093645E-5</v>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
@@ -1217,12 +1217,12 @@
         <v>1.8335666567127771</v>
       </c>
       <c r="L7" s="15">
-        <f t="shared" si="1"/>
-        <v>9.7397515923315907E-4</v>
+        <f t="shared" ref="L7:L11" si="1">(I7*1000)/E7</f>
+        <v>973.97515923315905</v>
       </c>
       <c r="M7" s="15">
         <f t="shared" si="0"/>
-        <v>1.9006030299093645E-5</v>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="8" spans="1:13" x14ac:dyDescent="0.25">
@@ -1261,11 +1261,11 @@
       </c>
       <c r="L8" s="15">
         <f t="shared" si="1"/>
-        <v>9.7397515923315907E-4</v>
+        <v>973.97515923315905</v>
       </c>
       <c r="M8" s="15">
         <f t="shared" si="0"/>
-        <v>1.9006030299093645E-5</v>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.25">
@@ -1304,11 +1304,11 @@
       </c>
       <c r="L9" s="15">
         <f t="shared" si="1"/>
-        <v>8.130054802589125E-4</v>
+        <v>813.00548025891248</v>
       </c>
       <c r="M9" s="15">
         <f t="shared" si="0"/>
-        <v>1.9006030299093642E-5</v>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.25">
@@ -1347,11 +1347,11 @@
       </c>
       <c r="L10" s="15">
         <f t="shared" si="1"/>
-        <v>8.130054802589125E-4</v>
+        <v>813.00548025891248</v>
       </c>
       <c r="M10" s="15">
         <f t="shared" si="0"/>
-        <v>1.9006030299093642E-5</v>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.25">
@@ -1390,11 +1390,11 @@
       </c>
       <c r="L11" s="15">
         <f t="shared" si="1"/>
-        <v>8.130054802589125E-4</v>
+        <v>813.00548025891248</v>
       </c>
       <c r="M11" s="15">
         <f t="shared" si="0"/>
-        <v>1.9006030299093642E-5</v>
+        <v>19.006030299093645</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.25">
@@ -11814,7 +11814,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D20" sqref="D20"/>
     </sheetView>
   </sheetViews>

</xml_diff>